<commit_message>
updated the controller, now constructing patients from the excel database
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,19 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>yes</t>
+    <t>a</t>
   </si>
   <si>
-    <t>hello</t>
+    <t>bbb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -58,8 +57,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,25 +361,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>12.33</v>
+      </c>
+      <c r="D1">
+        <v>1.22</v>
+      </c>
+      <c r="E1">
+        <v>1.22</v>
+      </c>
+      <c r="F1">
+        <v>12.31</v>
+      </c>
+      <c r="G1">
+        <v>12.43</v>
+      </c>
+      <c r="H1">
+        <v>543.20000000000005</v>
+      </c>
+      <c r="I1">
+        <v>123.43</v>
+      </c>
+      <c r="J1">
+        <v>54.23</v>
+      </c>
+      <c r="K1">
+        <v>134.21</v>
+      </c>
+      <c r="L1">
+        <v>1111.2</v>
+      </c>
+      <c r="M1" s="1">
+        <v>42445.895833333336</v>
+      </c>
+      <c r="N1" s="1">
+        <v>42445.895833333336</v>
+      </c>
+      <c r="O1" s="1">
+        <v>42445.895833333336</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+      <c r="C2">
+        <v>12.33</v>
+      </c>
+      <c r="D2">
+        <v>1.22</v>
+      </c>
+      <c r="E2">
+        <v>1.22</v>
+      </c>
+      <c r="F2">
+        <v>12.31</v>
+      </c>
+      <c r="G2">
+        <v>12.43</v>
+      </c>
+      <c r="H2">
+        <v>543.20000000000005</v>
+      </c>
+      <c r="I2">
+        <v>123.43</v>
+      </c>
+      <c r="J2">
+        <v>54.23</v>
+      </c>
+      <c r="K2">
+        <v>134.21</v>
+      </c>
+      <c r="L2">
+        <v>1111.2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>42445.895833333336</v>
+      </c>
+      <c r="N2" s="1">
+        <v>42445.895833333336</v>
+      </c>
+      <c r="O2" s="1">
+        <v>42445.895833333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added two more panels, reading from database to display
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>a</t>
+    <t>ahmed</t>
   </si>
   <si>
-    <t>bbb</t>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>menna</t>
   </si>
 </sst>
 </file>
@@ -57,9 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,18 +368,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="13" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -418,13 +426,19 @@
       <c r="O1" s="1">
         <v>42445.895833333336</v>
       </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>12.33</v>
@@ -464,10 +478,17 @@
       </c>
       <c r="O2" s="1">
         <v>42445.895833333336</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add patient now woriking, delete is "work in progress", tweaked database interfacing
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="6">
   <si>
     <t>ahmed</t>
   </si>
@@ -24,16 +24,26 @@
     <t>male</t>
   </si>
   <si>
+    <t>heba</t>
+  </si>
+  <si>
+    <t>hala</t>
+  </si>
+  <si>
     <t>female</t>
   </si>
   <si>
-    <t>menna</t>
+    <t>ss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy hh:mm"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,10 +73,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,122 +400,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="11.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1.0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>12.33</v>
-      </c>
-      <c r="D1">
-        <v>1.22</v>
-      </c>
-      <c r="E1">
-        <v>1.22</v>
-      </c>
-      <c r="F1">
-        <v>12.31</v>
-      </c>
-      <c r="G1">
-        <v>12.43</v>
-      </c>
-      <c r="H1">
-        <v>543.20000000000005</v>
-      </c>
-      <c r="I1">
-        <v>123.43</v>
-      </c>
-      <c r="J1">
-        <v>54.23</v>
-      </c>
-      <c r="K1">
-        <v>134.21</v>
-      </c>
-      <c r="L1">
-        <v>1111.2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>42445.895833333336</v>
-      </c>
-      <c r="N1" s="1">
-        <v>42445.895833333336</v>
-      </c>
-      <c r="O1" s="1">
-        <v>42445.895833333336</v>
+        <v>2</v>
+      </c>
+      <c r="M1" t="n" s="23">
+        <v>42457.05393122685</v>
       </c>
       <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="2">
-        <v>25</v>
+      <c r="Q1" t="n">
+        <v>44.0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2.0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>12.33</v>
-      </c>
-      <c r="D2">
-        <v>1.22</v>
-      </c>
-      <c r="E2">
-        <v>1.22</v>
-      </c>
-      <c r="F2">
-        <v>12.31</v>
-      </c>
-      <c r="G2">
-        <v>12.43</v>
-      </c>
-      <c r="H2">
-        <v>543.20000000000005</v>
-      </c>
-      <c r="I2">
-        <v>123.43</v>
-      </c>
-      <c r="J2">
-        <v>54.23</v>
-      </c>
-      <c r="K2">
-        <v>134.21</v>
-      </c>
-      <c r="L2">
-        <v>1111.2</v>
-      </c>
-      <c r="M2" s="1">
-        <v>42445.895833333336</v>
-      </c>
-      <c r="N2" s="1">
-        <v>42445.895833333336</v>
-      </c>
-      <c r="O2" s="1">
-        <v>42445.895833333336</v>
+        <v>5</v>
+      </c>
+      <c r="M2" t="n" s="24">
+        <v>42457.05393173611</v>
       </c>
       <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="n" s="22">
+        <v>42457.05386638889</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="n" s="14">
+        <v>42457.04991763889</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add and delete now working
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,33 +16,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="6">
-  <si>
-    <t>ahmed</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>male</t>
   </si>
   <si>
-    <t>heba</t>
+    <t>Ahmed</t>
   </si>
   <si>
-    <t>hala</t>
+    <t>menna</t>
   </si>
   <si>
     <t>female</t>
   </si>
   <si>
-    <t>ss</t>
+    <t>ibrahim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="d/m/yy hh:mm"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy hh:mm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -73,32 +71,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,49 +377,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="11.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="15.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1.0</v>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1">
+        <v>42457.065178784724</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="M1" t="n" s="23">
-        <v>42457.05393122685</v>
-      </c>
-      <c r="P1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" t="n">
-        <v>44.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2.0</v>
-      </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" t="n" s="24">
-        <v>42457.05393173611</v>
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>42457.065610300924</v>
       </c>
       <c r="P2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1.0</v>
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -450,33 +427,16 @@
         <v>3.0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" t="n" s="22">
-        <v>42457.05386638889</v>
+        <v>4</v>
+      </c>
+      <c r="M3" t="n" s="3">
+        <v>42457.06626491898</v>
       </c>
       <c r="P3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" t="n" s="14">
-        <v>42457.04991763889</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1.0</v>
+        <v>18.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit is now working
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>male</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>ibrahim</t>
+  </si>
+  <si>
+    <t>msel7y</t>
+  </si>
+  <si>
+    <t>ayaaaa</t>
   </si>
 </sst>
 </file>
@@ -71,10 +77,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -388,38 +400,38 @@
     <col min="13" max="13" customWidth="true" style="1" width="15.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1.0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1">
-        <v>42457.065178784724</v>
+      <c r="M1" t="n" s="7">
+        <v>42457.078729479166</v>
       </c>
       <c r="P1" t="s">
         <v>0</v>
       </c>
-      <c r="Q1">
-        <v>77</v>
+      <c r="Q1" t="n">
+        <v>77.0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2.0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2">
-        <v>42457.065610300924</v>
+        <v>5</v>
+      </c>
+      <c r="M2" t="n" s="8">
+        <v>42457.07872990741</v>
       </c>
       <c r="P2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>90.0</v>
       </c>
     </row>
     <row r="3">
@@ -427,16 +439,16 @@
         <v>3.0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" t="n" s="3">
-        <v>42457.06626491898</v>
+        <v>6</v>
+      </c>
+      <c r="M3" t="n" s="9">
+        <v>42457.07873026621</v>
       </c>
       <c r="P3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q3" t="n">
-        <v>18.0</v>
+        <v>22.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added alarm functionality (sound + animation)
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
   <si>
     <t>male</t>
   </si>
@@ -37,6 +37,36 @@
   </si>
   <si>
     <t>ayaaaa</t>
+  </si>
+  <si>
+    <t>shehab</t>
+  </si>
+  <si>
+    <t>shehab hany</t>
+  </si>
+  <si>
+    <t>mohammed</t>
+  </si>
+  <si>
+    <t>alaa</t>
+  </si>
+  <si>
+    <t>alaa kaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shehab </t>
+  </si>
+  <si>
+    <t>mina</t>
+  </si>
+  <si>
+    <t>aok</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>assss</t>
   </si>
 </sst>
 </file>
@@ -77,10 +107,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -405,16 +473,16 @@
         <v>1.0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" t="n" s="7">
-        <v>42457.078729479166</v>
+        <v>12</v>
+      </c>
+      <c r="M1" t="n" s="46">
+        <v>42473.67649376157</v>
       </c>
       <c r="P1" t="s">
         <v>0</v>
       </c>
       <c r="Q1" t="n">
-        <v>77.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="2">
@@ -422,32 +490,15 @@
         <v>2.0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" t="n" s="8">
-        <v>42457.07872990741</v>
+        <v>13</v>
+      </c>
+      <c r="M2" t="n" s="47">
+        <v>42473.67649424769</v>
       </c>
       <c r="P2" t="s">
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" t="n" s="9">
-        <v>42457.07873026621</v>
-      </c>
-      <c r="P3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="n">
         <v>22.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added blood type select box + functionality improvements
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -1,84 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="20112" windowHeight="7488"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Blood Type</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Date Modified</t>
+  </si>
+  <si>
+    <t>Heart Rate1</t>
+  </si>
+  <si>
+    <t>Heart Rate2</t>
+  </si>
+  <si>
+    <t>Heart Rate3</t>
+  </si>
+  <si>
+    <t>Heart Rate4</t>
+  </si>
+  <si>
+    <t>Heart Rate5</t>
+  </si>
+  <si>
+    <t>Temp1</t>
+  </si>
+  <si>
+    <t>Temp2</t>
+  </si>
+  <si>
+    <t>Temp3</t>
+  </si>
+  <si>
+    <t>Temp4</t>
+  </si>
+  <si>
+    <t>Temp5</t>
+  </si>
+  <si>
+    <t>Alarm</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
   <si>
     <t>male</t>
   </si>
   <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>menna</t>
+    <t>shehab</t>
+  </si>
+  <si>
+    <t>mayar</t>
+  </si>
+  <si>
+    <t>AB+</t>
   </si>
   <si>
     <t>female</t>
   </si>
   <si>
-    <t>ibrahim</t>
-  </si>
-  <si>
-    <t>msel7y</t>
-  </si>
-  <si>
-    <t>ayaaaa</t>
-  </si>
-  <si>
-    <t>shehab</t>
-  </si>
-  <si>
-    <t>shehab hany</t>
-  </si>
-  <si>
-    <t>mohammed</t>
-  </si>
-  <si>
-    <t>alaa</t>
-  </si>
-  <si>
-    <t>alaa kaka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shehab </t>
-  </si>
-  <si>
-    <t>mina</t>
-  </si>
-  <si>
-    <t>aok</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>assss</t>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>hamada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="d/m/yy\ hh:mm"/>
-    <numFmt numFmtId="166" formatCode="d/m/yy hh:mm"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="d/m/yy hh:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +119,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,70 +149,381 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="52">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A202" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <autoFilter ref="A1:A202"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="ID" dataDxfId="49"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="J1:J269" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="J1:J269"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Temp3" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="K1:K390" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="K1:K390"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Temp4" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="L1:L310" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="L1:L310"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Temp5" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table23" displayName="Table23" ref="M1:M444" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="M1:M444"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Blood Type" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="N1:N214" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="N1:N214"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Sex" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="O1:O237" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="O1:O237"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Age" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table26" displayName="Table26" ref="P1:P262" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="P1:P262"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Date Created" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table27" displayName="Table27" ref="Q1:R364" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="Q1:R364"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Date Modified" dataDxfId="1"/>
+    <tableColumn id="2" name="Alarm" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B1048576" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="B1:B1048576"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Name" dataDxfId="46"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C1:C324" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="C1:C324"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Heart Rate1" dataDxfId="43"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="D1:D105" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="D1:D105"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Heart Rate2" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="E1:E263" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="E1:E263"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Heart Rate3" dataDxfId="37"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="F1:F133" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="F1:F133"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Heart Rate4" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="G1:G277" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="G1:G277"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Heart Rate5" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="H1:H348" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="H1:H348"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Temp1" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="I1:I348" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="I1:I348"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Temp2" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,54 +813,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" customWidth="true" style="1" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="1" width="7.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
+    <col min="8" max="11" customWidth="true" style="6" width="9.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="6" width="9.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="13.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="7.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="7" width="6.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="9" width="20.77734375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="9" width="23.44140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="8" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="n" s="46">
-        <v>42473.67649376157</v>
-      </c>
-      <c r="P1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" t="n">
-        <v>24.0</v>
+      <c r="I1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="P2" t="n" s="24">
+        <v>42501.207151319446</v>
+      </c>
+      <c r="Q2" t="n" s="24">
+        <v>42501.22014013889</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2.0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="n" s="47">
-        <v>42473.67649424769</v>
-      </c>
-      <c r="P2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="n">
         <v>22.0</v>
+      </c>
+      <c r="P3" t="n" s="25">
+        <v>42501.22033280093</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="17">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Input is now working + updating the draw panels
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>hamada</t>
+  </si>
+  <si>
+    <t>Shehab</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -168,6 +171,8 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -910,10 +915,10 @@
       <c r="O2" t="n">
         <v>12.0</v>
       </c>
-      <c r="P2" t="n" s="24">
+      <c r="P2" t="n" s="26">
         <v>42501.207151319446</v>
       </c>
-      <c r="Q2" t="n" s="24">
+      <c r="Q2" t="n" s="26">
         <v>42501.22014013889</v>
       </c>
     </row>
@@ -922,19 +927,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
         <v>20</v>
       </c>
       <c r="O3" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="P3" t="n" s="25">
-        <v>42501.22033280093</v>
+        <v>25.0</v>
+      </c>
+      <c r="P3" t="n" s="27">
+        <v>42502.77497329861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added exception handling for message strings
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -72,47 +72,34 @@
     <t>Alarm</t>
   </si>
   <si>
-    <t>ahmed</t>
-  </si>
-  <si>
     <t>O+</t>
   </si>
   <si>
     <t>male</t>
   </si>
   <si>
-    <t>shehab</t>
-  </si>
-  <si>
-    <t>mayar</t>
-  </si>
-  <si>
-    <t>AB+</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
     <t>B-</t>
   </si>
   <si>
-    <t>hamada</t>
-  </si>
-  <si>
-    <t>Shehab</t>
+    <t>patient 1</t>
+  </si>
+  <si>
+    <t>patient 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
     <numFmt numFmtId="166" formatCode="0;[Red]0"/>
     <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm:ss"/>
-    <numFmt numFmtId="169" formatCode="d/m/yy hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -156,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -171,22 +158,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -821,26 +792,26 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="7.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="13.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
-    <col min="8" max="11" customWidth="true" style="6" width="9.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="6" width="9.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="13.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="2" width="7.44140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="7" width="6.44140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="9" width="20.77734375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="9" width="23.44140625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="8" width="22.6640625" collapsed="true"/>
+    <col min="1" max="1" width="7.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="11" width="9.44140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.5546875" style="6" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="7.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.44140625" style="7" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.77734375" style="9" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.44140625" style="9" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22.6640625" style="8" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -899,47 +870,50 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>12</v>
+      </c>
+      <c r="P2" s="10">
+        <v>42501.207151319446</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>42501.220140138888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3">
         <v>25</v>
       </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="P2" t="n" s="26">
-        <v>42501.207151319446</v>
-      </c>
-      <c r="Q2" t="n" s="26">
-        <v>42501.22014013889</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="P3" t="n" s="27">
-        <v>42502.77497329861</v>
+      <c r="P3" s="11">
+        <v>42502.774973298612</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>42515.659065601852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
writing 5 most recent values is now working
</commit_message>
<xml_diff>
--- a/src/data/control/patients.xlsx
+++ b/src/data/control/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -72,34 +72,47 @@
     <t>Alarm</t>
   </si>
   <si>
+    <t>ahmed</t>
+  </si>
+  <si>
     <t>O+</t>
   </si>
   <si>
     <t>male</t>
   </si>
   <si>
+    <t>shehab</t>
+  </si>
+  <si>
+    <t>mayar</t>
+  </si>
+  <si>
+    <t>AB+</t>
+  </si>
+  <si>
     <t>female</t>
   </si>
   <si>
     <t>B-</t>
   </si>
   <si>
-    <t>patient 1</t>
-  </si>
-  <si>
-    <t>patient 2</t>
+    <t>hamada</t>
+  </si>
+  <si>
+    <t>Shehab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000;[Red]0.0000"/>
     <numFmt numFmtId="166" formatCode="0;[Red]0"/>
     <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="d/m/yy hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -143,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -158,6 +171,24 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -792,26 +823,26 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="11" width="9.44140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.5546875" style="6" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="6.44140625" style="7" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.77734375" style="9" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.44140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="22.6640625" style="8" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="7.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
+    <col min="8" max="11" customWidth="true" style="6" width="9.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="6" width="9.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="13.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="7.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="7" width="6.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="9" width="20.77734375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="9" width="23.44140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="8" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -870,50 +901,107 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
+      <c r="C2" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>36.16999816894531</v>
+      </c>
+      <c r="I2" t="n">
+        <v>36.70000076293945</v>
+      </c>
+      <c r="J2" t="n">
+        <v>35.709999084472656</v>
+      </c>
+      <c r="K2" t="n">
+        <v>35.70000076293945</v>
+      </c>
+      <c r="L2" t="n">
+        <v>36.900001525878906</v>
+      </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="P2" t="n" s="28">
+        <v>42501.207151319446</v>
+      </c>
+      <c r="Q2" t="n" s="28">
+        <v>42501.22014013889</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>35.86000061035156</v>
+      </c>
+      <c r="I3" t="n">
+        <v>35.77000045776367</v>
+      </c>
+      <c r="J3" t="n">
+        <v>37.09000015258789</v>
+      </c>
+      <c r="K3" t="n">
+        <v>37.029998779296875</v>
+      </c>
+      <c r="L3" t="n">
+        <v>36.0099983215332</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>20</v>
       </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-      <c r="P2" s="10">
-        <v>42501.207151319446</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>42501.220140138888</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3">
-        <v>25</v>
-      </c>
-      <c r="P3" s="11">
-        <v>42502.774973298612</v>
-      </c>
-      <c r="Q3" s="11">
-        <v>42515.659065601852</v>
+      <c r="O3" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="P3" t="n" s="29">
+        <v>42502.77497329861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>